<commit_message>
Updated the DataLoadManager, added 3 and 4 days
</commit_message>
<xml_diff>
--- a/REport-Please.xlsx
+++ b/REport-Please.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donatas Vaiciulis\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donc3 Kebabas\Documents\GitHub\Report_Please\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9C61EB-C6DF-4594-9C9A-3029886BCA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F16CA5-C6CE-497F-AF8E-FE3A62244A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="765" windowWidth="22920" windowHeight="14340" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1005" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descrepancy fields" sheetId="1" r:id="rId1"/>
@@ -647,29 +647,6 @@
     <t>REPORTS ARE TESTED ON ALL LATEST VERSIONS</t>
   </si>
   <si>
-    <t>CASE ID: 1542164
-Unity: Physics2D
-TESTER: David
-DESKTOP GRABBAG
-Collision geometry is not applied correctly to a Tilemap when Composite Collider's 2D "Geometry Type" is set to Polygons
-How to reproduce:
-1.  Open the user's attached "TileCollisionBug.zip" project 
-2. Open the "SampleScene" Scene (Assets folder)
-3. Make sure the Scene view is visible
-4. Select the "Tilemap" GameObject in the Hierarchy window
-5. Observe the Scene view
-Expected result: Correct collision geometry is applied to the Tilemap, no tiles are left without a collider and there are no holes in the collider
-Actual result: Two colliders appear on the Tilemap, as the Tilemap gets wider the collider gets more inconsistent 
-eventually leaving a hole in the center of the Tilemap
-Reproducible with: 2018.4.27f1, 2019.4.11f1, 2020.1.6f1, 2020.2.0b3
-REGRESSION: NO
-FAV: 2018.4, 2020.2
-PUBLIC: YES
-SEVERITY: 3
-PLATFORM - 3
-USER - 2</t>
-  </si>
-  <si>
     <t>BAD REPORT 
 WRONG GRABBAG
 TEMPLATE USED:
@@ -739,32 +716,6 @@
   </si>
   <si>
     <t>ENTERPRISE BUG REPORTS SHOULD NOT BE RESPONDED</t>
-  </si>
-  <si>
-    <t>CASE ID: 1791012
-Unity: Scene Management
-TESTER DONNY
-SCENE MANAGEMENT GRABBAG
-Multi-selecting and overwriting Prefab instances with changes does not apply changes to their outside Prefab assets
-How to reproduce:
-1. Open the user's attached "Bug Project.zip" project
-2. Open the "SampleScene" Scene
-3. Type "t:boxcollider" in the Hierarchy window's search bar
-4. Select all GameObjects in the Hierarchy window
-5. Remove the Box Collider Component in the Inspector
-6. Clear the search bar
-7. Select all parent GameObjects in the Hierarchy window
-8. Press Overrides -&gt; Apply All in the Inspector window
-9. Observe the GameObjects in the Scene view
-Expected result: Box Collider Component was removed from all Prefab instances and from the original Prefab
-Actual result: On some Prefab instances and on the original Prefab, the Box Collider Component was not removed, but on some of the Prefab instances it was removed
-Reproducible with: 2018.4.27f1, 2019.4.11f1, 2020.1.6f1
-REGRESION: NO
-FAV: 2018.4, 2020.1
-PUBLIC YES
-SEVEIRY 3
-PLATFORM 3
-USER 2</t>
   </si>
   <si>
     <t>BAD REPORT
@@ -1027,6 +978,53 @@
 PACKAGE Shader Graph
 PACKAGE FOUND VERSION 10.0.0-preview.27
 </t>
+  </si>
+  <si>
+    <t>CASE ID: 1542164
+Unity: Physics2D
+TESTER: David
+The 2D Guy
+Collision geometry is not applied correctly to a Tilemap when Composite Collider's 2D "Geometry Type" is set to Polygons
+How to reproduce:
+1.  Open the user's attached "TileCollisionBug.zip" project 
+2. Open the "SampleScene" Scene (Assets folder)
+3. Make sure the Scene view is visible
+4. Select the "Tilemap" GameObject in the Hierarchy window
+5. Observe the Scene view
+Expected result: Correct collision geometry is applied to the Tilemap, no tiles are left without a collider and there are no holes in the collider
+Actual result: Two colliders appear on the Tilemap, as the Tilemap gets wider the collider gets more inconsistent 
+eventually leaving a hole in the center of the Tilemap
+Reproducible with: 2018.4.27f1, 2019.4.11f1, 2020.1.6f1, 2020.2.0b3
+REGRESSION: NO
+FAV: 2018.4, 2020.2
+PUBLIC: YES
+SEVERITY: 3
+PLATFORM - 3
+USER - 2</t>
+  </si>
+  <si>
+    <t>CASE ID: 1791012
+Unity: Scene Management
+TESTER DONNY
+SCENE MANAGEMENT GRABBAG
+Multi-selecting and overwriting Prefab instances with changes does not apply changes to their outside Prefab assets
+How to reproduce:
+1. Open the user's attached "Bug Project.zip" project
+2. Type "t:boxcollider" in the Hierarchy window's search bar
+3. Select all GameObjects in the Hierarchy window
+4. Remove the Box Collider Component in the Inspector
+5. Select all parent GameObjects in the Hierarchy window
+6. Press Overrides -&gt; Apply All in the Inspector window
+7. Observe the GameObjects in the Scene view
+Expected result: Box Collider Component was removed from all Prefab instances and from the original Prefab
+Actual result: On some Prefab instances and on the original Prefab, the Box Collider Component was not removed, but on some of the Prefab instances it was removed
+Reproducible with: 2018.4.27f1, 2019.4.11f1, 2020.1.6f1
+REGRESION: NO
+FAV: 2018.4, 2020.1
+PUBLIC YES
+SEVEIRY 3
+PLATFORM 3
+USER 2</t>
   </si>
 </sst>
 </file>
@@ -1899,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF5E72D-022D-46FA-AEEC-2C52C59856C0}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,90 +1916,90 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>119</v>
-      </c>
       <c r="C2" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
@@ -2247,7 +2245,7 @@
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="3"/>
@@ -3021,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C167742A-2883-4BB6-9224-D481EC052D8D}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3249,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C85F19-1EB9-48E8-AC8B-37E2EB2B2563}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,15 +3306,15 @@
     </row>
     <row r="6" spans="1:3" ht="252" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="252" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" s="13"/>
     </row>
@@ -3465,8 +3463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B1A98A-F854-4130-A0C3-A739ECB8580F}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,7 +3493,7 @@
         <v>95</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
@@ -3556,18 +3554,18 @@
     </row>
     <row r="10" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="330" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Home page for Rule Book, updated the classes to be without Unity
</commit_message>
<xml_diff>
--- a/REport-Please.xlsx
+++ b/REport-Please.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donc3 Kebabas\Documents\GitHub\Report_Please\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2934133-BF3C-4E28-88EA-854E2BCEC311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1F3ABF-0D07-4CC4-A3DD-14B751AC88DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="1860" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="780" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descrepancy fields" sheetId="1" r:id="rId1"/>
@@ -1189,10 +1189,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1523,46 +1523,46 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -1794,19 +1794,71 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
@@ -1823,71 +1875,19 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2150,40 +2150,40 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -2198,72 +2198,72 @@
       <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -2447,6 +2447,49 @@
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A7:F7"/>
@@ -2463,49 +2506,6 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2806,13 +2806,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E13:F13"/>
@@ -2821,6 +2814,13 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3019,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C167742A-2883-4BB6-9224-D481EC052D8D}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,7 +3463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B1A98A-F854-4130-A0C3-A739ECB8580F}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Field Checker and Citations work for Day 3
Day 4 is left
</commit_message>
<xml_diff>
--- a/REport-Please.xlsx
+++ b/REport-Please.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donc3 Kebabas\Documents\GitHub\Report_Please\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1F3ABF-0D07-4CC4-A3DD-14B751AC88DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B7BFFC-E2F9-4AC0-A411-61FA50FD9A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="780" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11310" yWindow="1365" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descrepancy fields" sheetId="1" r:id="rId1"/>
@@ -1189,10 +1189,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1523,46 +1523,46 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -1794,36 +1794,54 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -1840,54 +1858,36 @@
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2150,40 +2150,40 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -2198,72 +2198,72 @@
       <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -2447,49 +2447,6 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A7:F7"/>
@@ -2506,6 +2463,49 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2806,6 +2806,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E13:F13"/>
@@ -2814,13 +2821,6 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3019,7 +3019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C167742A-2883-4BB6-9224-D481EC052D8D}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3463,8 +3463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B1A98A-F854-4130-A0C3-A739ECB8580F}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Started working on Day 4 Checker
Needs fixing
</commit_message>
<xml_diff>
--- a/REport-Please.xlsx
+++ b/REport-Please.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donc3 Kebabas\Documents\GitHub\Report_Please\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B7BFFC-E2F9-4AC0-A411-61FA50FD9A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF017DB7-73E0-43AB-8684-FD81640284BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11310" yWindow="1365" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="10275" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descrepancy fields" sheetId="1" r:id="rId1"/>
@@ -1189,10 +1189,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1523,46 +1523,46 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -1794,19 +1794,71 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
@@ -1823,71 +1875,19 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1897,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF5E72D-022D-46FA-AEEC-2C52C59856C0}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,40 +2150,40 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -2198,72 +2198,72 @@
       <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -2447,6 +2447,49 @@
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A7:F7"/>
@@ -2463,49 +2506,6 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2806,13 +2806,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E13:F13"/>
@@ -2821,6 +2814,13 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3463,8 +3463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B1A98A-F854-4130-A0C3-A739ECB8580F}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished checker for all days
</commit_message>
<xml_diff>
--- a/REport-Please.xlsx
+++ b/REport-Please.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donc3 Kebabas\Documents\GitHub\Report_Please\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF017DB7-73E0-43AB-8684-FD81640284BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCBE5CF-BED9-4777-9925-146999A3BCBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="10275" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6405" yWindow="1605" windowWidth="21600" windowHeight="13305" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descrepancy fields" sheetId="1" r:id="rId1"/>
@@ -1189,10 +1189,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1523,46 +1523,46 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -1794,36 +1794,54 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -1840,54 +1858,36 @@
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1897,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF5E72D-022D-46FA-AEEC-2C52C59856C0}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,40 +2150,40 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
@@ -2198,72 +2198,72 @@
       <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -2447,49 +2447,6 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A7:F7"/>
@@ -2506,6 +2463,49 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2806,6 +2806,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E13:F13"/>
@@ -2814,13 +2821,6 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3463,8 +3463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B1A98A-F854-4130-A0C3-A739ECB8580F}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>